<commit_message>
Redesign the data preprocessing pipeline, use min-max-rescale as the normalization, use normal distribution as the standardization
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{BB095D5E-2162-4C52-85D1-9866AA1C5AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB87ECEF-E9CC-4A49-98A7-255E5834E241}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{BB095D5E-2162-4C52-85D1-9866AA1C5AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6E47509-4F03-4617-B915-5CF624E99EFD}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="240" windowWidth="29040" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="17">
   <si>
     <t>1000</t>
   </si>
@@ -425,7 +425,7 @@
   <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -441,7 +441,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="2">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2">
         <v>20</v>
@@ -461,8 +461,8 @@
       <c r="I1" s="2">
         <v>1600</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>0</v>
+      <c r="J1" s="2">
+        <v>1</v>
       </c>
       <c r="K1">
         <v>1.2</v>

</xml_diff>